<commit_message>
Added new members, added own time spend
</commit_message>
<xml_diff>
--- a/Time schedule.xlsx
+++ b/Time schedule.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solomon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas\Documents\GitHub\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0DE126-CB9A-436F-940C-990872A3C336}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="Week 9" sheetId="12" r:id="rId10"/>
     <sheet name="Total" sheetId="4" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -180,11 +179,20 @@
   <si>
     <t>did my part for the project plan</t>
   </si>
+  <si>
+    <t>Prepare meeting client</t>
+  </si>
+  <si>
+    <t>Artem Dvoiiakovskyi</t>
+  </si>
+  <si>
+    <t>Mukhitdin Iakhiarov</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -562,13 +570,15 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -647,11 +657,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -928,11 +940,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,13 +1423,19 @@
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="43" t="s">
         <v>25</v>
       </c>
       <c r="O20" s="7">
@@ -1427,12 +1445,18 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
       <c r="N21" s="43" t="s">
         <v>37</v>
       </c>
@@ -1443,13 +1467,20 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1498,13 +1529,19 @@
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="43" t="s">
         <v>25</v>
       </c>
       <c r="O24" s="7">
@@ -1514,32 +1551,44 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="41" t="s">
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="O25" s="42">
+      <c r="O25" s="44">
         <v>0.25</v>
       </c>
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="41" t="s">
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="42">
+      <c r="O26" s="44">
         <v>0.25</v>
       </c>
       <c r="P26" s="5"/>
@@ -1584,6 +1633,163 @@
       <c r="P27" s="6">
         <f>SUM(C27:O27)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="C29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="C30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="C33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1593,11 +1799,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,6 +2414,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2215,11 +2635,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2698,7 @@
       </c>
       <c r="D2" s="25">
         <f>'Week 2'!P7</f>
-        <v>4.75</v>
+        <v>6.75</v>
       </c>
       <c r="E2" s="25">
         <f>'Week 3'!P7</f>
@@ -2310,7 +2730,7 @@
       </c>
       <c r="L2" s="29">
         <f>SUM(B2:K2)</f>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2358,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="30">
-        <f t="shared" ref="L3:L7" si="0">SUM(B3:K3)</f>
+        <f t="shared" ref="L3:L5" si="0">SUM(B3:K3)</f>
         <v>1.55</v>
       </c>
     </row>
@@ -2505,57 +2925,155 @@
         <v>0</v>
       </c>
       <c r="L6" s="30">
-        <f t="shared" si="0"/>
+        <f>SUM(B6:K6)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53" t="s">
+    <row r="7" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="9">
         <f>'Week 1'!P27</f>
         <v>1</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="26">
         <f>'May Vacation'!P27</f>
         <v>1.5</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="26">
         <f>'Week 2'!P27</f>
         <v>0</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="26">
         <f>'Week 3'!P27</f>
         <v>0</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="26">
         <f>'Week 4'!P27</f>
         <v>0</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="26">
         <f>'Week 5'!P27</f>
         <v>0</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="26">
         <f>'Week 6'!P27</f>
         <v>0</v>
       </c>
-      <c r="I7" s="46">
+      <c r="I7" s="26">
         <f>'Week 7'!P27</f>
         <v>0</v>
       </c>
-      <c r="J7" s="46">
+      <c r="J7" s="26">
         <f>'Week 8'!P27</f>
         <v>0</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="44">
         <f>'Week 9'!P27</f>
         <v>0</v>
       </c>
-      <c r="L7" s="31">
-        <f t="shared" si="0"/>
+      <c r="L7" s="30">
+        <f>SUM(B7:K7)</f>
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9">
+        <f>'Week 1'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="26">
+        <f>'May Vacation'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
+        <f>'Week 2'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="26">
+        <f>'Week 3'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="26">
+        <f>'Week 4'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="26">
+        <f>'Week 5'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="26">
+        <f>'Week 6'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="26">
+        <f>'Week 7'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="26">
+        <f>'Week 8'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="44">
+        <f>'Week 9'!P31</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="30">
+        <f t="shared" ref="L8:L9" si="1">SUM(B8:K8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="45">
+        <f>'Week 1'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="46">
+        <f>'May Vacation'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="46">
+        <f>'Week 2'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="46">
+        <f>'Week 3'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="46">
+        <f>'Week 4'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="46">
+        <f>'Week 5'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="46">
+        <f>'Week 6'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="46">
+        <f>'Week 7'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="46">
+        <f>'Week 8'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="47">
+        <f>'Week 9'!P35</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2564,11 +3082,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,7 +3099,7 @@
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="29" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3128,7 +3646,9 @@
       <c r="N24" t="s">
         <v>45</v>
       </c>
-      <c r="O24" s="7"/>
+      <c r="O24" s="7">
+        <v>1.5</v>
+      </c>
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3189,12 +3709,227 @@
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="4">
+        <f>SUM(O24:O26)</f>
         <v>1.5</v>
       </c>
       <c r="P27" s="6">
         <f>SUM(C27:O27)</f>
         <v>1.5</v>
       </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3203,11 +3938,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,9 +3952,9 @@
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -3355,9 +4090,20 @@
       <c r="G4" s="8">
         <v>0.25</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="H4" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.5</v>
+      </c>
       <c r="K4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="43"/>
       <c r="O4" s="7"/>
       <c r="P4" s="5"/>
     </row>
@@ -3378,7 +4124,12 @@
       </c>
       <c r="I5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="44">
+        <v>1</v>
+      </c>
       <c r="O5" s="8"/>
       <c r="P5" s="5"/>
     </row>
@@ -3394,7 +4145,8 @@
       </c>
       <c r="I6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="44"/>
       <c r="O6" s="8"/>
       <c r="P6" s="5"/>
     </row>
@@ -3418,7 +4170,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="4">
         <f>SUM(I4:I6)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="4">
@@ -3428,7 +4180,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="4">
         <f>SUM(M4:M6)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="4">
@@ -3437,7 +4189,7 @@
       </c>
       <c r="P7" s="6">
         <f>SUM(C7:O7)</f>
-        <v>4.75</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3850,6 +4602,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3857,11 +4823,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4472,6 +5438,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4479,11 +5659,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,6 +6274,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5101,11 +6495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5716,6 +7110,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5723,11 +7331,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6338,6 +7946,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6345,11 +8167,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6960,6 +8782,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6967,11 +9003,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:P27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A28" sqref="A28:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7582,6 +9618,220 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4">
+        <f>SUM(C28:C30)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <f>SUM(E28:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4">
+        <f>SUM(K28:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4">
+        <f>SUM(M28:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4">
+        <f>SUM(O28:O30)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <f>SUM(C31:O31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4">
+        <f>SUM(C32:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <f>SUM(E32:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4">
+        <f>SUM(G32:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4">
+        <f>SUM(I32:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <f>SUM(K32:K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="3"/>
+      <c r="M35" s="4">
+        <f>SUM(M32:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4">
+        <f>SUM(O32:O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="6">
+        <f>SUM(C35:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>